<commit_message>
created and added interlex identifiers
</commit_message>
<xml_diff>
--- a/aibs-patchseq/curated/allele_resources.xlsx
+++ b/aibs-patchseq/curated/allele_resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia\Documents\Work\NWB\ontology-project\aibs-patchseq\curated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F20977-3E9C-43CF-A981-26AADC6AFBBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA65852B-7897-4F72-8D51-A8BFC555F3E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19335" yWindow="2775" windowWidth="37665" windowHeight="22710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29565" yWindow="6270" windowWidth="35895" windowHeight="22710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allele" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="269">
   <si>
     <t>Vip-IRES-Cre</t>
   </si>
@@ -744,21 +744,12 @@
     <t>ncbigene:269132</t>
   </si>
   <si>
-    <t>cre</t>
-  </si>
-  <si>
     <t>FLP</t>
   </si>
   <si>
     <t>tdTomato</t>
   </si>
   <si>
-    <t>cre/ERT2</t>
-  </si>
-  <si>
-    <t>expressed_gene_symbol</t>
-  </si>
-  <si>
     <t>allele_symbol</t>
   </si>
   <si>
@@ -771,14 +762,89 @@
     <t>EGFP</t>
   </si>
   <si>
-    <t>EGFP/cre</t>
+    <t>dgCre</t>
+  </si>
+  <si>
+    <t>CreERT2</t>
+  </si>
+  <si>
+    <t>Cre</t>
+  </si>
+  <si>
+    <t>ILX:0102616</t>
+  </si>
+  <si>
+    <t>ILX:0516968</t>
+  </si>
+  <si>
+    <t>ILX:0778019</t>
+  </si>
+  <si>
+    <t>ILX:0778020</t>
+  </si>
+  <si>
+    <t>expressed_protein_symbol</t>
+  </si>
+  <si>
+    <t>expressed_protein_url</t>
+  </si>
+  <si>
+    <t>ILX:0778021</t>
+  </si>
+  <si>
+    <t>ILX:0103825</t>
+  </si>
+  <si>
+    <t>RRID:MMRRC_036504-UCD</t>
+  </si>
+  <si>
+    <t>jaxmice:009111</t>
+  </si>
+  <si>
+    <t>MGI:3838497</t>
+  </si>
+  <si>
+    <t>Tg(Scnn1a-cre)1Aibs </t>
+  </si>
+  <si>
+    <t>Transgene</t>
+  </si>
+  <si>
+    <t>Tg(Nr5a1-cre)2Lowl</t>
+  </si>
+  <si>
+    <t>Tg(Gad1-EGFP)94Agmo</t>
+  </si>
+  <si>
+    <t>Tg(Slc17a8-icre)1Edw </t>
+  </si>
+  <si>
+    <t>TIGRE</t>
+  </si>
+  <si>
+    <t>MGI:5490612</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>ChrR-tdT</t>
+  </si>
+  <si>
+    <t>ILX:0778022</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>ILX:0778023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -931,6 +997,18 @@
       <sz val="10"/>
       <color rgb="FF000001"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF72C02C"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1288,7 +1366,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1316,6 +1394,14 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1363,7 +1449,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1423,27 +1512,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L54" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="allele_symbol" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="stock_identifier" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="stock_url" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M55" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:M55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="allele_symbol" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="stock_identifier" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="stock_url" dataDxfId="10">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="allele_identifier" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="allele_generation_method" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="allele_attributes" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="allele_url" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="allele_identifier" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="allele_generation_method" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="allele_attributes" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="allele_url" dataDxfId="6">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="locus_symbol" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="locus_identifier" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="locus_type" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="locus_url" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="locus_symbol" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="locus_identifier" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="locus_type" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="locus_url" dataDxfId="2">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{49EB3C91-816B-450F-8EC3-0F8269484BB8}" name="expressed_gene_symbol" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{49EB3C91-816B-450F-8EC3-0F8269484BB8}" name="expressed_protein_symbol" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{B298A87F-912C-457C-95FF-C69913345255}" name="expressed_protein_url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1746,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,14 +1855,15 @@
     <col min="10" max="10" width="16.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="35.140625" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>135</v>
@@ -1790,7 +1881,7 @@
         <v>60</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>62</v>
@@ -1802,10 +1893,13 @@
         <v>66</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1843,10 +1937,13 @@
         <v>https://identifiers.org/ncbigene:22353</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1884,10 +1981,13 @@
         <v>https://identifiers.org/ncbigene:14910</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1925,10 +2025,13 @@
         <v>https://identifiers.org/ncbigene:20604</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1966,10 +2069,13 @@
         <v>https://identifiers.org/ncbigene:22355</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2007,10 +2113,13 @@
         <v>https://identifiers.org/ncbigene:22348</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2048,10 +2157,13 @@
         <v>https://identifiers.org/ncbigene:14910</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2089,10 +2201,13 @@
         <v>https://identifiers.org/ncbigene:12647</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2130,10 +2245,13 @@
         <v>https://identifiers.org/ncbigene:19293</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2171,10 +2289,13 @@
         <v>https://identifiers.org/ncbigene:110902</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2212,10 +2333,13 @@
         <v>https://identifiers.org/ncbigene:18430</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2253,10 +2377,13 @@
         <v>https://identifiers.org/ncbigene:15561</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2294,10 +2421,13 @@
         <v>https://identifiers.org/ncbigene:225998</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2335,10 +2465,13 @@
         <v>https://identifiers.org/ncbigene:22348</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2376,10 +2509,13 @@
         <v>https://identifiers.org/ncbigene:14417</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2417,10 +2553,13 @@
         <v>https://identifiers.org/ncbigene:18125</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2458,10 +2597,13 @@
         <v>https://identifiers.org/ncbigene:20604</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2499,10 +2641,13 @@
         <v>https://identifiers.org/ncbigene:68169</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2540,10 +2685,13 @@
         <v>https://identifiers.org/ncbigene:18610</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2567,18 +2715,27 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
         <v>https://identifiers.org/MGI:3617314</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="7" t="str">
-        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
-        <v>https://identifiers.org/</v>
+      <c r="H20" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="K20" s="9" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
+        <v>https://identifiers.org/MGI:3617314</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2616,10 +2773,13 @@
         <v>https://identifiers.org/ncbigene:216227</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -2657,10 +2817,13 @@
         <v>https://identifiers.org/ncbigene:22348</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -2698,10 +2861,13 @@
         <v>https://identifiers.org/ncbigene:19662</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2739,10 +2905,13 @@
         <v>https://identifiers.org/ncbigene:12918</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2780,10 +2949,13 @@
         <v>https://identifiers.org/ncbigene:21333</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -2821,10 +2993,13 @@
         <v>https://identifiers.org/ncbigene:13048</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -2862,10 +3037,13 @@
         <v>https://identifiers.org/ncbigene:14910</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -2903,10 +3081,13 @@
         <v>https://identifiers.org/ncbigene:18216</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -2944,10 +3125,13 @@
         <v>https://identifiers.org/ncbigene:12308</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -2985,10 +3169,13 @@
         <v>https://identifiers.org/ncbigene:19293</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -3026,10 +3213,13 @@
         <v>https://identifiers.org/ncbigene:21823</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -3067,10 +3257,13 @@
         <v>https://identifiers.org/ncbigene:140919</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -3108,10 +3301,13 @@
         <v>https://identifiers.org/ncbigene:18162</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -3149,10 +3345,13 @@
         <v>https://identifiers.org/ncbigene:72961</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -3190,10 +3389,13 @@
         <v>https://identifiers.org/ncbigene:22353</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M35" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -3231,10 +3433,13 @@
         <v>https://identifiers.org/ncbigene:14009</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="M36" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -3272,10 +3477,13 @@
         <v>https://identifiers.org/ncbigene:21869</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>36</v>
       </c>
@@ -3299,10 +3507,13 @@
         <v>https://identifiers.org/</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -3326,18 +3537,27 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
         <v>https://identifiers.org/MGI:5316477</v>
       </c>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="7" t="str">
-        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
-        <v>https://identifiers.org/</v>
+      <c r="H39" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="K39" s="9" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
+        <v>https://identifiers.org/MGI:5316477</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -3375,10 +3595,13 @@
         <v>https://identifiers.org/ncbigene:109648</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M40" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -3402,18 +3625,27 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
         <v>https://identifiers.org/MGI:3697310</v>
       </c>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="7" t="str">
-        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
-        <v>https://identifiers.org/</v>
+      <c r="H41" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="K41" s="9" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
+        <v>https://identifiers.org/MGI:3697310</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -3451,10 +3683,13 @@
         <v>https://identifiers.org/ncbigene:19293</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="M42" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -3492,17 +3727,22 @@
         <v>https://identifiers.org/ncbigene:12424</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7" t="str">
-        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
-        <v>https://identifiers.org/</v>
+      <c r="B44" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C44" s="9" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
+        <v>https://identifiers.org/RRID:MMRRC_036504-UCD</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>234</v>
@@ -3531,10 +3771,13 @@
         <v>https://identifiers.org/ncbigene:269132</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -3572,10 +3815,13 @@
         <v>https://identifiers.org/ncbigene:18619</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M45" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -3613,10 +3859,13 @@
         <v>https://identifiers.org/ncbigene:140919</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M46" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
@@ -3632,16 +3881,27 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
         <v>https://identifiers.org/</v>
       </c>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="7" t="str">
-        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
-        <v>https://identifiers.org/</v>
-      </c>
-      <c r="L47" s="6"/>
-    </row>
-    <row r="48" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="H47" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="K47" s="9" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
+        <v>https://identifiers.org/MGI:5490612</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="M47" s="14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -3679,17 +3939,20 @@
         <v>https://identifiers.org/ncbigene:27140</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="M48" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C49" s="4" t="str">
+      <c r="C49" s="7" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
         <v>https://identifiers.org/jaxmice:034424</v>
       </c>
@@ -3708,30 +3971,57 @@
         <v>https://identifiers.org/</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="M49" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B50" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="C50" s="4" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
-        <v>https://identifiers.org/</v>
+        <v>https://identifiers.org/jaxmice:009111</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="G50" s="4" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
-        <v>https://identifiers.org/</v>
+        <v>https://identifiers.org/MGI:3838497</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
-        <v>https://identifiers.org/</v>
+        <v>https://identifiers.org/MGI:3838497</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M50" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
@@ -3754,9 +4044,14 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/</v>
       </c>
-      <c r="L51" s="6"/>
-    </row>
-    <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L51" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="M51" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
@@ -3765,19 +4060,28 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
         <v>https://identifiers.org/</v>
       </c>
-      <c r="G52" s="4" t="str">
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="7" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
         <v>https://identifiers.org/</v>
       </c>
-      <c r="K52" s="4" t="str">
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="7" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M52" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -3815,10 +4119,13 @@
         <v>https://identifiers.org/ncbigene:13983</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="M53" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -3855,9 +4162,34 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/ncbigene:14219</v>
       </c>
-      <c r="L54" s="6" t="s">
-        <v>246</v>
-      </c>
+      <c r="L54" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="M54" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C55" s="15" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G55" s="15" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778023</v>
+      </c>
+      <c r="K55" s="15" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
example notebook to chain together all the csv file information
</commit_message>
<xml_diff>
--- a/aibs-patchseq/curated/allele_resources.xlsx
+++ b/aibs-patchseq/curated/allele_resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia\Documents\Work\NWB\ontology-project\aibs-patchseq\curated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA65852B-7897-4F72-8D51-A8BFC555F3E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AAC217-F609-4209-B4F1-2CFDAA18E647}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29565" yWindow="6270" windowWidth="35895" windowHeight="22710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="3060" windowWidth="46080" windowHeight="23415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allele" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="280">
   <si>
     <t>Vip-IRES-Cre</t>
   </si>
@@ -783,12 +783,6 @@
     <t>ILX:0778020</t>
   </si>
   <si>
-    <t>expressed_protein_symbol</t>
-  </si>
-  <si>
-    <t>expressed_protein_url</t>
-  </si>
-  <si>
     <t>ILX:0778021</t>
   </si>
   <si>
@@ -838,6 +832,45 @@
   </si>
   <si>
     <t>ILX:0778023</t>
+  </si>
+  <si>
+    <t>recombinase_symbol</t>
+  </si>
+  <si>
+    <t>recombinase_url</t>
+  </si>
+  <si>
+    <t>recombinase_identifier</t>
+  </si>
+  <si>
+    <t>reporter_symbol</t>
+  </si>
+  <si>
+    <t>reporter_identifier</t>
+  </si>
+  <si>
+    <t>reporter_url</t>
+  </si>
+  <si>
+    <t>promotor_symbol</t>
+  </si>
+  <si>
+    <t>CAG</t>
+  </si>
+  <si>
+    <t>LSL</t>
+  </si>
+  <si>
+    <t>TRE2 </t>
+  </si>
+  <si>
+    <t>FSF-LSL</t>
+  </si>
+  <si>
+    <t>FSF</t>
+  </si>
+  <si>
+    <t>expression_controller_symbol</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1399,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1403,6 +1436,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1449,7 +1484,20 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1512,28 +1560,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M55" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="allele_symbol" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="stock_identifier" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="stock_url" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:S55" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:S55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="allele_symbol" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="stock_identifier" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="stock_url" dataDxfId="14">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="allele_identifier" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="allele_generation_method" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="allele_attributes" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="allele_url" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="allele_identifier" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="allele_generation_method" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="allele_attributes" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="allele_url" dataDxfId="10">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="locus_symbol" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="locus_identifier" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="locus_type" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="locus_url" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="locus_symbol" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="locus_identifier" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="locus_type" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="locus_url" dataDxfId="6">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{49EB3C91-816B-450F-8EC3-0F8269484BB8}" name="expressed_protein_symbol" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{B298A87F-912C-457C-95FF-C69913345255}" name="expressed_protein_url" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{39722E5E-9919-4486-BD60-B371C0C85BAF}" name="recombinase_symbol"/>
+    <tableColumn id="15" xr3:uid="{A72C865F-50C7-43DB-89C1-5511F9A8BAE8}" name="recombinase_identifier"/>
+    <tableColumn id="17" xr3:uid="{5881D34C-6869-4B58-829D-07D0566408C0}" name="recombinase_url" dataDxfId="1">
+      <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{49EB3C91-816B-450F-8EC3-0F8269484BB8}" name="reporter_symbol" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{B298A87F-912C-457C-95FF-C69913345255}" name="reporter_identifier" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{F42F75E9-9FD8-4A79-AB3B-75E85E9D4BB7}" name="reporter_url" dataDxfId="0">
+      <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{AFC506A0-C416-4FF1-9701-C876ACB738B1}" name="promotor_symbol" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{FB7556F9-84F5-4438-AC27-3EBBF01F3DF4}" name="expression_controller_symbol" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1836,29 +1894,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="34.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="35.140625" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="18.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="34.54296875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.7265625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.7265625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.26953125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="35.1796875" customWidth="1"/>
+    <col min="12" max="14" width="16.7265625" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="16" width="13.26953125" customWidth="1"/>
+    <col min="17" max="17" width="15.81640625" customWidth="1"/>
+    <col min="18" max="18" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>239</v>
       </c>
@@ -1893,13 +1954,31 @@
         <v>66</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1942,8 +2021,20 @@
       <c r="M2" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N2" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1980,14 +2071,30 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/ncbigene:14910</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q3" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778019</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2030,8 +2137,20 @@
       <c r="M4" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N4" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2074,8 +2193,20 @@
       <c r="M5" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N5" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2118,8 +2249,20 @@
       <c r="M6" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N6" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2156,14 +2299,30 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/ncbigene:14910</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="2"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="P7" s="13" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q7" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778019</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2206,8 +2365,20 @@
       <c r="M8" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N8" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2250,8 +2421,20 @@
       <c r="M9" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N9" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2294,8 +2477,20 @@
       <c r="M10" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N10" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2338,8 +2533,20 @@
       <c r="M11" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N11" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2382,8 +2589,20 @@
       <c r="M12" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N12" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2426,8 +2645,20 @@
       <c r="M13" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N13" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2470,8 +2701,20 @@
       <c r="M14" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N14" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2514,8 +2757,20 @@
       <c r="M15" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N15" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2556,10 +2811,22 @@
         <v>244</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="N16" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778021</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2602,8 +2869,20 @@
       <c r="M17" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N17" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2646,8 +2925,20 @@
       <c r="M18" s="13" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N18" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778020</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2688,10 +2979,22 @@
         <v>244</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="N19" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778021</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2716,13 +3019,13 @@
         <v>https://identifiers.org/MGI:3617314</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>154</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K20" s="9" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
@@ -2734,8 +3037,20 @@
       <c r="M20" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N20" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2778,8 +3093,20 @@
       <c r="M21" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N21" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -2822,8 +3149,20 @@
       <c r="M22" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N22" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -2866,8 +3205,20 @@
       <c r="M23" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N23" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+    </row>
+    <row r="24" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2910,8 +3261,20 @@
       <c r="M24" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N24" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+    </row>
+    <row r="25" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2954,8 +3317,20 @@
       <c r="M25" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N25" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+    </row>
+    <row r="26" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -2996,10 +3371,22 @@
         <v>244</v>
       </c>
       <c r="M26" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="N26" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778021</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+    </row>
+    <row r="27" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -3036,14 +3423,30 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/ncbigene:14910</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="2"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="O27" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="M27" s="13" t="s">
+      <c r="P27" s="13" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q27" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778019</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -3086,8 +3489,20 @@
       <c r="M28" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N28" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+    </row>
+    <row r="29" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -3130,8 +3545,20 @@
       <c r="M29" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N29" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+    </row>
+    <row r="30" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -3174,8 +3601,20 @@
       <c r="M30" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N30" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+    </row>
+    <row r="31" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -3218,8 +3657,20 @@
       <c r="M31" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N31" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+    </row>
+    <row r="32" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -3262,8 +3713,20 @@
       <c r="M32" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N32" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+    </row>
+    <row r="33" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -3306,8 +3769,20 @@
       <c r="M33" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N33" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+    </row>
+    <row r="34" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -3350,8 +3825,20 @@
       <c r="M34" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N34" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+    </row>
+    <row r="35" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -3394,8 +3881,20 @@
       <c r="M35" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N35" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+    </row>
+    <row r="36" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -3436,10 +3935,22 @@
         <v>244</v>
       </c>
       <c r="M36" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="N36" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778021</v>
+      </c>
+      <c r="O36" s="2"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+    </row>
+    <row r="37" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -3480,10 +3991,22 @@
         <v>244</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="N37" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778021</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+    </row>
+    <row r="38" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>36</v>
       </c>
@@ -3512,8 +4035,20 @@
       <c r="M38" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N38" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+    </row>
+    <row r="39" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -3538,13 +4073,13 @@
         <v>https://identifiers.org/MGI:5316477</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>205</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K39" s="9" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
@@ -3556,8 +4091,20 @@
       <c r="M39" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N39" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+    </row>
+    <row r="40" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -3600,8 +4147,20 @@
       <c r="M40" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N40" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O40" s="2"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+    </row>
+    <row r="41" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -3626,26 +4185,38 @@
         <v>https://identifiers.org/MGI:3697310</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>232</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K41" s="9" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/MGI:3697310</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="L41" s="2"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="O41" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="M41" s="13" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="P41" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q41" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0103825</v>
+      </c>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+    </row>
+    <row r="42" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -3686,10 +4257,22 @@
         <v>244</v>
       </c>
       <c r="M42" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="N42" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778021</v>
+      </c>
+      <c r="O42" s="2"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+    </row>
+    <row r="43" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -3732,13 +4315,25 @@
       <c r="M43" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N43" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O43" s="2"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+    </row>
+    <row r="44" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C44" s="9" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
@@ -3776,8 +4371,20 @@
       <c r="M44" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N44" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O44" s="2"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+    </row>
+    <row r="45" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -3820,8 +4427,20 @@
       <c r="M45" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N45" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O45" s="2"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+    </row>
+    <row r="46" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -3864,8 +4483,20 @@
       <c r="M46" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N46" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O46" s="2"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+    </row>
+    <row r="47" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
@@ -3882,26 +4513,40 @@
         <v>https://identifiers.org/</v>
       </c>
       <c r="H47" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="J47" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="K47" s="9" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
+        <v>https://identifiers.org/MGI:5490612</v>
+      </c>
+      <c r="L47" s="8"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="17" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="O47" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="J47" s="8" t="s">
+      <c r="P47" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="K47" s="9" t="str">
-        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
-        <v>https://identifiers.org/MGI:5490612</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="M47" s="14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q47" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778022</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="S47" s="2"/>
+    </row>
+    <row r="48" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -3944,8 +4589,20 @@
       <c r="M48" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N48" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+    </row>
+    <row r="49" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
@@ -3976,20 +4633,32 @@
       <c r="M49" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N49" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O49" s="2"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+    </row>
+    <row r="50" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C50" s="4" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
         <v>https://identifiers.org/jaxmice:009111</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>123</v>
@@ -4002,13 +4671,13 @@
         <v>https://identifiers.org/MGI:3838497</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I50" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
@@ -4020,8 +4689,20 @@
       <c r="M50" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N50" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+    </row>
+    <row r="51" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
@@ -4050,8 +4731,20 @@
       <c r="M51" s="13" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N51" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0516968</v>
+      </c>
+      <c r="O51" s="8"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+    </row>
+    <row r="52" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
@@ -4080,8 +4773,20 @@
       <c r="M52" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N52" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O52" s="2"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+    </row>
+    <row r="53" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -4124,8 +4829,20 @@
       <c r="M53" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N53" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0102616</v>
+      </c>
+      <c r="O53" s="2"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+    </row>
+    <row r="54" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -4168,17 +4885,29 @@
       <c r="M54" s="13" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N54" s="16" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778020</v>
+      </c>
+      <c r="O54" s="8"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+    </row>
+    <row r="55" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C55" s="15" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</f>
         <v>https://identifiers.org/</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G55" s="15" t="str">
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</f>
@@ -4188,8 +4917,20 @@
         <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</f>
         <v>https://identifiers.org/</v>
       </c>
-      <c r="L55" s="2"/>
+      <c r="L55" s="15"/>
       <c r="M55" s="2"/>
+      <c r="N55" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added recombinase, promoter, expression_controller identifiers
</commit_message>
<xml_diff>
--- a/aibs-patchseq/curated/allele_resources.xlsx
+++ b/aibs-patchseq/curated/allele_resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia\Documents\Work\NWB\ontology-project\aibs-patchseq\curated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AAC217-F609-4209-B4F1-2CFDAA18E647}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7708378-ACBC-432F-9EB4-3FF00A8F313D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4605" yWindow="3060" windowWidth="46080" windowHeight="23415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="7185" windowWidth="53385" windowHeight="23415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allele" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="289">
   <si>
     <t>Vip-IRES-Cre</t>
   </si>
@@ -852,9 +852,6 @@
     <t>reporter_url</t>
   </si>
   <si>
-    <t>promotor_symbol</t>
-  </si>
-  <si>
     <t>CAG</t>
   </si>
   <si>
@@ -871,6 +868,36 @@
   </si>
   <si>
     <t>expression_controller_symbol</t>
+  </si>
+  <si>
+    <t>ILX:0778025</t>
+  </si>
+  <si>
+    <t>ILX:0778026</t>
+  </si>
+  <si>
+    <t>promoter_symbol</t>
+  </si>
+  <si>
+    <t>promoter_identifier</t>
+  </si>
+  <si>
+    <t>promoter_url</t>
+  </si>
+  <si>
+    <t>ILX:0778027</t>
+  </si>
+  <si>
+    <t>ILX:0778028</t>
+  </si>
+  <si>
+    <t>expression_controller_identifier</t>
+  </si>
+  <si>
+    <t>expression_controller_url</t>
+  </si>
+  <si>
+    <t>ILX:0778029</t>
   </si>
 </sst>
 </file>
@@ -1484,15 +1511,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="23">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1502,7 +1523,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1560,38 +1601,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:S55" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:S55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="allele_symbol" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="stock_identifier" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="stock_url" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:W55" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:W55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="allele_symbol" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="stock_identifier" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="stock_url" dataDxfId="18">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[stock_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="allele_identifier" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="allele_generation_method" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="allele_attributes" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="allele_url" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="allele_identifier" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="allele_generation_method" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="allele_attributes" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="allele_url" dataDxfId="14">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[allele_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="locus_symbol" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="locus_identifier" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="locus_type" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="locus_url" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="locus_symbol" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="locus_identifier" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="locus_type" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="locus_url" dataDxfId="10">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[locus_identifier]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" xr3:uid="{39722E5E-9919-4486-BD60-B371C0C85BAF}" name="recombinase_symbol"/>
     <tableColumn id="15" xr3:uid="{A72C865F-50C7-43DB-89C1-5511F9A8BAE8}" name="recombinase_identifier"/>
-    <tableColumn id="17" xr3:uid="{5881D34C-6869-4B58-829D-07D0566408C0}" name="recombinase_url" dataDxfId="1">
+    <tableColumn id="17" xr3:uid="{5881D34C-6869-4B58-829D-07D0566408C0}" name="recombinase_url" dataDxfId="9">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[recombinase_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{49EB3C91-816B-450F-8EC3-0F8269484BB8}" name="reporter_symbol" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{B298A87F-912C-457C-95FF-C69913345255}" name="reporter_identifier" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{F42F75E9-9FD8-4A79-AB3B-75E85E9D4BB7}" name="reporter_url" dataDxfId="0">
+    <tableColumn id="12" xr3:uid="{49EB3C91-816B-450F-8EC3-0F8269484BB8}" name="reporter_symbol" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{B298A87F-912C-457C-95FF-C69913345255}" name="reporter_identifier" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{F42F75E9-9FD8-4A79-AB3B-75E85E9D4BB7}" name="reporter_url" dataDxfId="6">
       <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[reporter_identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{AFC506A0-C416-4FF1-9701-C876ACB738B1}" name="promotor_symbol" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{AFC506A0-C416-4FF1-9701-C876ACB738B1}" name="promoter_symbol" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{CE293C44-8B38-4E63-9FE5-EC557D7DDCCF}" name="promoter_identifier" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{7C36D6B0-F8C1-485F-B484-74F27976AB6B}" name="promoter_url" dataDxfId="3">
+      <calculatedColumnFormula>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="20" xr3:uid="{FB7556F9-84F5-4438-AC27-3EBBF01F3DF4}" name="expression_controller_symbol" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{99D726A3-51E9-49A6-8E2B-848CBBCDC45E}" name="expression_controller_identifier" dataDxfId="1"/>
+    <tableColumn id="26" xr3:uid="{1F15E801-E994-413B-9532-9D5FE9C8BAA6}" name="expression_controller_url" dataDxfId="0">
+      <calculatedColumnFormula>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1894,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S55"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1916,10 +1965,10 @@
     <col min="15" max="15" width="19" customWidth="1"/>
     <col min="16" max="16" width="13.26953125" customWidth="1"/>
     <col min="17" max="17" width="15.81640625" customWidth="1"/>
-    <col min="18" max="18" width="17.90625" customWidth="1"/>
+    <col min="18" max="20" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>239</v>
       </c>
@@ -1972,13 +2021,25 @@
         <v>272</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2033,8 +2094,18 @@
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
+      <c r="T2" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2088,13 +2159,27 @@
         <v>https://identifiers.org/ILX:0778019</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="T3" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778025</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>275</v>
+      <c r="V3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="W3" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/ILX:0778027</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2149,8 +2234,18 @@
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
+      <c r="T4" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2205,8 +2300,18 @@
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
+      <c r="T5" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2261,8 +2366,18 @@
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
+      <c r="T6" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2316,13 +2431,27 @@
         <v>https://identifiers.org/ILX:0778019</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
+      </c>
+      <c r="T7" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778025</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="W7" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/ILX:0778029</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2377,8 +2506,18 @@
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
+      <c r="T8" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2433,8 +2572,18 @@
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
+      <c r="T9" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2489,8 +2638,18 @@
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
+      <c r="T10" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2545,8 +2704,18 @@
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
+      <c r="T11" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2601,8 +2770,18 @@
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
+      <c r="T12" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2657,8 +2836,18 @@
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
+      <c r="T13" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2713,8 +2902,18 @@
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
+      <c r="T14" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2769,8 +2968,18 @@
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
+      <c r="T15" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2825,8 +3034,18 @@
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
+      <c r="T16" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2881,8 +3100,18 @@
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
+      <c r="T17" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2937,8 +3166,18 @@
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
+      <c r="T18" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2993,8 +3232,18 @@
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
+      <c r="T19" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -3049,8 +3298,18 @@
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
+      <c r="T20" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -3105,8 +3364,18 @@
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
+      <c r="T21" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="22" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -3161,8 +3430,18 @@
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
+      <c r="T22" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="23" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -3217,8 +3496,18 @@
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
+      <c r="T23" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="24" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -3273,8 +3562,18 @@
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
+      <c r="T24" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="25" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -3329,8 +3628,18 @@
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
+      <c r="T25" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="26" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -3385,8 +3694,18 @@
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
+      <c r="T26" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="27" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -3440,13 +3759,27 @@
         <v>https://identifiers.org/ILX:0778019</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
+      </c>
+      <c r="T27" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778025</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="V27" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="W27" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/ILX:0778028</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -3501,8 +3834,18 @@
       </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
+      <c r="T28" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="29" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -3557,8 +3900,18 @@
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
+      <c r="T29" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="30" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -3613,8 +3966,18 @@
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
+      <c r="T30" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="31" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -3669,8 +4032,18 @@
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
+      <c r="T31" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="32" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -3725,8 +4098,18 @@
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
+      <c r="T32" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="33" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -3781,8 +4164,18 @@
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
+      <c r="T33" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="34" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -3837,8 +4230,18 @@
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
+      <c r="T34" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="35" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -3893,8 +4296,18 @@
       </c>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
+      <c r="T35" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="36" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -3949,8 +4362,18 @@
       </c>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
+      <c r="T36" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="37" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -4005,8 +4428,18 @@
       </c>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
+      <c r="T37" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="38" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>36</v>
       </c>
@@ -4047,8 +4480,18 @@
       </c>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
+      <c r="T38" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="39" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -4103,8 +4546,18 @@
       </c>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
+      <c r="T39" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="40" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4159,8 +4612,18 @@
       </c>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
+      <c r="T40" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="41" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -4215,8 +4678,18 @@
       </c>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
+      <c r="T41" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="42" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -4271,8 +4744,18 @@
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
+      <c r="T42" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="43" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -4327,8 +4810,18 @@
       </c>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
+      <c r="T43" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="44" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -4383,8 +4876,18 @@
       </c>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
+      <c r="T44" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="45" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -4439,8 +4942,18 @@
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
+      <c r="T45" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="46" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -4495,8 +5008,18 @@
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
+      <c r="T46" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="47" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
@@ -4542,11 +5065,23 @@
         <v>https://identifiers.org/ILX:0778022</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="S47" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="T47" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/ILX:0778026</v>
+      </c>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="48" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -4601,8 +5136,18 @@
       </c>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
+      <c r="T48" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="49" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
@@ -4645,8 +5190,18 @@
       </c>
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
+      <c r="T49" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="50" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -4701,8 +5256,18 @@
       </c>
       <c r="R50" s="2"/>
       <c r="S50" s="2"/>
+      <c r="T50" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="51" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
@@ -4743,8 +5308,18 @@
       </c>
       <c r="R51" s="2"/>
       <c r="S51" s="2"/>
+      <c r="T51" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="52" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
@@ -4785,8 +5360,18 @@
       </c>
       <c r="R52" s="2"/>
       <c r="S52" s="2"/>
+      <c r="T52" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="53" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -4841,8 +5426,18 @@
       </c>
       <c r="R53" s="2"/>
       <c r="S53" s="2"/>
+      <c r="T53" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U53" s="2"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="54" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -4897,8 +5492,18 @@
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
+      <c r="T54" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
-    <row r="55" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>265</v>
       </c>
@@ -4931,6 +5536,16 @@
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
+      <c r="T55" s="4" t="str">
+        <f>HYPERLINK("https://identifiers.org/"&amp;Table1[[#This Row],[promoter_identifier]])</f>
+        <v>https://identifiers.org/</v>
+      </c>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="4" t="str">
+        <f>HYPERLINK("https:/identifiers.org/"&amp;Table1[[#This Row],[expression_controller_identifier]])</f>
+        <v>https:/identifiers.org/</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>